<commit_message>
Update weather and dose to 7.5 kg/t
</commit_message>
<xml_diff>
--- a/2021-0294106_digestate_NH3_EFs/inputs/inputs.xlsx
+++ b/2021-0294106_digestate_NH3_EFs/inputs/inputs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Slurry" sheetId="1" state="visible" r:id="rId2"/>
@@ -48,7 +48,7 @@
     <t xml:space="preserve">2.1 kg/t</t>
   </si>
   <si>
-    <t xml:space="preserve">5.7 kg/t</t>
+    <t xml:space="preserve">7.5 kg/t</t>
   </si>
   <si>
     <t xml:space="preserve">app.timing.dk</t>
@@ -112,10 +112,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -190,7 +191,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -208,6 +209,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -290,8 +295,8 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -370,8 +375,8 @@
         <v>5.1</v>
       </c>
       <c r="D5" s="4" t="n">
-        <f aca="false">7.9-1.01</f>
-        <v>6.89</v>
+        <f aca="false">7.9-1.11</f>
+        <v>6.79</v>
       </c>
     </row>
   </sheetData>
@@ -392,8 +397,8 @@
   </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -430,14 +435,14 @@
       <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>4.025</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>0.09</v>
+      <c r="C2" s="5" t="n">
+        <v>4.43101207056639</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>4.05891613991413</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>0.0599629009095261</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -447,14 +452,14 @@
       <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1" t="n">
-        <v>8.5</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>3.91</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>0.09</v>
+      <c r="C3" s="5" t="n">
+        <v>8.23645983645984</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>3.84445591865745</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>0.0552119412831931</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -464,14 +469,14 @@
       <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="1" t="n">
-        <v>12.4</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>3.565</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>0.09</v>
+      <c r="C4" s="5" t="n">
+        <v>12.4492495309568</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>3.48391526295633</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>0.0702993488962998</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -481,14 +486,14 @@
       <c r="B5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="1" t="n">
-        <v>16.867</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>3.18167</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>0.09</v>
+      <c r="C5" s="5" t="n">
+        <v>16.8762259816193</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>3.15624012423227</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>0.105925308296069</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -498,14 +503,14 @@
       <c r="B6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="1" t="n">
-        <v>14.6</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>3.45</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <v>0.09</v>
+      <c r="C6" s="5" t="n">
+        <v>14.4977479635841</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>3.32276959833633</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>0.128260170445409</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add 6.9% as additional DM input (keep 5.1%)
</commit_message>
<xml_diff>
--- a/2021-0294106_digestate_NH3_EFs/inputs/inputs.xlsx
+++ b/2021-0294106_digestate_NH3_EFs/inputs/inputs.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t xml:space="preserve">man.source</t>
   </si>
@@ -293,10 +293,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -375,6 +375,65 @@
         <v>5.1</v>
       </c>
       <c r="D5" s="4" t="n">
+        <f aca="false">7.9-1.11</f>
+        <v>6.79</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <f aca="false">7.9-1.38</f>
+        <v>6.52</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="D8" s="4" t="n">
+        <f aca="false">7.9-0.71</f>
+        <v>7.19</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="D9" s="4" t="n">
         <f aca="false">7.9-1.11</f>
         <v>6.79</v>
       </c>

</xml_diff>

<commit_message>
Update delta pH for 3.4 kg/t dose
</commit_message>
<xml_diff>
--- a/2021-0294106_digestate_NH3_EFs/inputs/inputs.xlsx
+++ b/2021-0294106_digestate_NH3_EFs/inputs/inputs.xlsx
@@ -296,7 +296,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -360,8 +360,8 @@
         <v>5.1</v>
       </c>
       <c r="D4" s="4" t="n">
-        <f aca="false">7.9-0.71</f>
-        <v>7.19</v>
+        <f aca="false">7.9-0.8187</f>
+        <v>7.0813</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -419,8 +419,8 @@
         <v>6.9</v>
       </c>
       <c r="D8" s="4" t="n">
-        <f aca="false">7.9-0.71</f>
-        <v>7.19</v>
+        <f aca="false">7.9-0.8187</f>
+        <v>7.0813</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Switch to digestate 5.9% DM n = 26
</commit_message>
<xml_diff>
--- a/2021-0294106_digestate_NH3_EFs/inputs/inputs.xlsx
+++ b/2021-0294106_digestate_NH3_EFs/inputs/inputs.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t xml:space="preserve">man.source</t>
   </si>
@@ -293,10 +293,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -328,7 +328,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>5.1</v>
+        <v>5.9</v>
       </c>
       <c r="D2" s="3" t="n">
         <v>7.9</v>
@@ -342,7 +342,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>5.1</v>
+        <v>5.9</v>
       </c>
       <c r="D3" s="4" t="n">
         <f aca="false">7.9-1.38</f>
@@ -357,7 +357,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>5.1</v>
+        <v>5.9</v>
       </c>
       <c r="D4" s="4" t="n">
         <f aca="false">7.9-0.8187</f>
@@ -372,68 +372,9 @@
         <v>8</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>5.1</v>
+        <v>5.9</v>
       </c>
       <c r="D5" s="4" t="n">
-        <f aca="false">7.9-1.11</f>
-        <v>6.79</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>6.9</v>
-      </c>
-      <c r="D6" s="3" t="n">
-        <v>7.9</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>6.9</v>
-      </c>
-      <c r="D7" s="4" t="n">
-        <f aca="false">7.9-1.38</f>
-        <v>6.52</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v>6.9</v>
-      </c>
-      <c r="D8" s="4" t="n">
-        <f aca="false">7.9-0.8187</f>
-        <v>7.0813</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>6.9</v>
-      </c>
-      <c r="D9" s="4" t="n">
         <f aca="false">7.9-1.11</f>
         <v>6.79</v>
       </c>

</xml_diff>

<commit_message>
Add 2 more DM levels to show variation in output.
</commit_message>
<xml_diff>
--- a/2021-0294106_digestate_NH3_EFs/inputs/inputs.xlsx
+++ b/2021-0294106_digestate_NH3_EFs/inputs/inputs.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
   <si>
     <t xml:space="preserve">man.source</t>
   </si>
@@ -293,10 +293,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -328,7 +328,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>5.9</v>
+        <v>5.1</v>
       </c>
       <c r="D2" s="3" t="n">
         <v>7.9</v>
@@ -342,7 +342,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>5.9</v>
+        <v>5.1</v>
       </c>
       <c r="D3" s="4" t="n">
         <f aca="false">7.9-1.38</f>
@@ -357,7 +357,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>5.9</v>
+        <v>5.1</v>
       </c>
       <c r="D4" s="4" t="n">
         <f aca="false">7.9-0.8187</f>
@@ -372,9 +372,127 @@
         <v>8</v>
       </c>
       <c r="C5" s="1" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <f aca="false">7.9-1.11</f>
+        <v>6.79</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="n">
         <v>5.9</v>
       </c>
-      <c r="D5" s="4" t="n">
+      <c r="D6" s="3" t="n">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <f aca="false">7.9-1.38</f>
+        <v>6.52</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="D8" s="4" t="n">
+        <f aca="false">7.9-0.8187</f>
+        <v>7.0813</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="D9" s="4" t="n">
+        <f aca="false">7.9-1.11</f>
+        <v>6.79</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="D10" s="3" t="n">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="D11" s="4" t="n">
+        <f aca="false">7.9-1.38</f>
+        <v>6.52</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="D12" s="4" t="n">
+        <f aca="false">7.9-0.8187</f>
+        <v>7.0813</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="D13" s="4" t="n">
         <f aca="false">7.9-1.11</f>
         <v>6.79</v>
       </c>

</xml_diff>